<commit_message>
update for ai response
</commit_message>
<xml_diff>
--- a/data/Report_format_2.xlsx
+++ b/data/Report_format_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhammad Al-Amin\Desktop\Al-Amin\llama_parse_al\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Al-Amin\llama_parse_al\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3472936B-94E5-41FD-AB8F-B18D77AE72B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE5BD83-095C-4047-A24B-43C15C3A670A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -36,90 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>The saturation of the lower glass point Xiaoli Pill is 65%</t>
   </si>
   <si>
-    <t>The upper and lower glass bonding saturation is 67.5%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>The saturation of amplified pills and sports cars is 73.3%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Silicone oil saturation 50.7%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Silicone oil port sealing + dispensing + curing saturation 58%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set Conn &amp; lower cover + paste QR CODE saturation 41%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lock the lid + label the saturation 81.7%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Glass module test saturation 100%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Visual inspection of UV glue + pull tape is the bottleneck station</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Measuring oil leakage is the bottleneck station</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>The next glass point Xiaoli Pill exists in Renwai Machine 2S</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dispensing UV glue, UV curing &amp; checking the existence of human machine 22S</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>The sum of the saturations of two adjacent processes is less than or equal to 95%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Production line balance rate 75.2%</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Low job saturation(lower than95%)</t>
   </si>
   <si>
     <t>Bottom glass electrophoresis tank+UVFixed baking operation saturation79.2%</t>
   </si>
   <si>
-    <t>Xiaoliwan wax+Paste conductive foam+Lower glass glue frame dispensing operation saturation75%</t>
-  </si>
-  <si>
-    <t>Five-in-one front&amp;back saturation53.2%</t>
-  </si>
-  <si>
-    <t>CellstickFPCsaturation61.9%</t>
-  </si>
-  <si>
-    <t>FPCFoam resistance test saturation40.8%</t>
-  </si>
-  <si>
-    <t>pointUVglue,UVsolidify&amp;Check saturation33.3%</t>
-  </si>
-  <si>
-    <t>Electrophoresis tank noteBufferliquid saturation79.2%</t>
-  </si>
-  <si>
-    <t>BufferLiquid injection port sealing and solidification+Water leakage test saturation60.3%</t>
-  </si>
-  <si>
     <t>Improvement Parameters</t>
   </si>
   <si>
@@ -145,21 +72,6 @@
   </si>
   <si>
     <t>Expected completion date</t>
-  </si>
-  <si>
-    <t>Job saturation 100%</t>
-  </si>
-  <si>
-    <t>Bottleneck station (the average C/T of the station is the largest)</t>
-  </si>
-  <si>
-    <t>Simultaneous working time of man and machine = manual time (39S) + automatic time (2S) - process standard C/T (41S) = 0S Time of man waiting for machine = automatic time (2S) - simultaneous working time of man and machine (0S) = 2S</t>
-  </si>
-  <si>
-    <t>The sum of Sn process saturation and S(n+1) process saturation is less than or equal to 95%</t>
-  </si>
-  <si>
-    <t>Balance rate is less than 90%</t>
   </si>
   <si>
     <t>Improvement direction</t>
@@ -317,7 +229,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -343,15 +255,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -361,6 +264,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,18 +284,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -663,17 +566,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6ABEA31-CD59-49E7-AF39-9ED29D7C6B98}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1252,53 +1155,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>39</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
@@ -1306,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="4"/>
@@ -1320,10 +1223,10 @@
     </row>
     <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
@@ -1335,346 +1238,6 @@
       <c r="J4" s="4"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:11" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="8"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="8"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="8"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A2"/>

</xml_diff>